<commit_message>
registeUser function checked successfully
</commit_message>
<xml_diff>
--- a/src/test/java/MainAssignment/UserDetails.xlsx
+++ b/src/test/java/MainAssignment/UserDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhamkumar32\IdeaProjects\restAssured\src\test\java\MainAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CB5F4B-A5FC-4A3C-8474-49E054554ADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EB81FE-3B09-477D-BA04-F0C2C7E42D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -40,15 +40,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>Shubham</t>
-  </si>
-  <si>
-    <t>shubham@gmail.com</t>
-  </si>
-  <si>
-    <t>shu123</t>
-  </si>
-  <si>
     <t>task</t>
   </si>
   <si>
@@ -110,6 +101,12 @@
   </si>
   <si>
     <t>add_task_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shubham kumar</t>
+  </si>
+  <si>
+    <t>shubhamk@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -446,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,13 +470,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>12345678</v>
       </c>
       <c r="D2">
         <v>22</v>
@@ -498,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928C1E34-CEAC-45B0-9FE4-3C200CD01998}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -509,107 +506,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login function added and working but adding tasks is not working
</commit_message>
<xml_diff>
--- a/src/test/java/MainAssignment/UserDetails.xlsx
+++ b/src/test/java/MainAssignment/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhamkumar32\IdeaProjects\restAssured\src\test\java\MainAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EB81FE-3B09-477D-BA04-F0C2C7E42D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8379FA-5E07-4C93-99C1-C23923CB8503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,10 +103,10 @@
     <t>add_task_20</t>
   </si>
   <si>
-    <t xml:space="preserve"> shubham kumar</t>
-  </si>
-  <si>
     <t>shubhamk@gmail.com</t>
+  </si>
+  <si>
+    <t>shubham kumar</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,10 +470,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>12345678</v>

</xml_diff>

<commit_message>
adding negative login case
</commit_message>
<xml_diff>
--- a/src/test/java/MainAssignment/UserDetails.xlsx
+++ b/src/test/java/MainAssignment/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhamkumar32\IdeaProjects\restAssured\src\test\java\MainAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8379FA-5E07-4C93-99C1-C23923CB8503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDAD9BC-87CD-4675-92FF-EE62A6C387BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
     <col min="2" max="2" width="28.81640625" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" customWidth="1"/>
   </cols>

</xml_diff>